<commit_message>
sort and export dashboard
</commit_message>
<xml_diff>
--- a/public/documents/Unconfirmed-Revit.xlsx
+++ b/public/documents/Unconfirmed-Revit.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15" count="15">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="95" count="95">
   <x:si>
     <x:t>name</x:t>
   </x:si>
@@ -349,6 +349,30 @@
     <x:t>WK980065</x:t>
   </x:si>
   <x:si>
+    <x:t>Dave Pratikkumar Jayeshbhai</x:t>
+  </x:si>
+  <x:si>
+    <x:t>9978921363</x:t>
+  </x:si>
+  <x:si>
+    <x:t>140373109023</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ELECTRICAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>pratik.dave90@ymail.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PARUL INSTITUTE OF ENGINEERING &amp; TECHNOLOGY</x:t>
+  </x:si>
+  <x:si>
+    <x:t>WK204529</x:t>
+  </x:si>
+  <x:si>
     <x:t>Parekh Dhaval Balkrishna</x:t>
   </x:si>
   <x:si>
@@ -575,6 +599,27 @@
   </x:si>
   <x:si>
     <x:t>WK481934</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Shah Pooja Sanjaybhai</x:t>
+  </x:si>
+  <x:si>
+    <x:t>9825964113</x:t>
+  </x:si>
+  <x:si>
+    <x:t>130800106042</x:t>
+  </x:si>
+  <x:si>
+    <x:t>080</x:t>
+  </x:si>
+  <x:si>
+    <x:t>shahpooja277@gmail.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>VADODARA INSTITUTE OF ENGINEERING</x:t>
+  </x:si>
+  <x:si>
+    <x:t>WK506034</x:t>
   </x:si>
   <x:si>
     <x:t>DABHI KISHAN</x:t>
@@ -1426,157 +1471,157 @@
         <x:v>114</x:v>
       </x:c>
       <x:c r="E18" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="F18" s="0" t="s">
-        <x:v>115</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="G18" s="0" t="s">
-        <x:v>65</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="H18" s="0" t="s">
-        <x:v>116</x:v>
+        <x:v>118</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:8">
       <x:c r="A19" s="0" t="s">
-        <x:v>117</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>118</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="C19" s="0" t="s">
-        <x:v>119</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
-        <x:v>120</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="E19" s="0" t="s">
         <x:v>63</x:v>
       </x:c>
       <x:c r="F19" s="0" t="s">
-        <x:v>121</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="G19" s="0" t="s">
-        <x:v>122</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="H19" s="0" t="s">
-        <x:v>123</x:v>
+        <x:v>124</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:8">
       <x:c r="A20" s="0" t="s">
-        <x:v>124</x:v>
+        <x:v>125</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>125</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="C20" s="0" t="s">
-        <x:v>126</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
-        <x:v>127</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="E20" s="0" t="s">
-        <x:v>71</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="F20" s="0" t="s">
-        <x:v>128</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="G20" s="0" t="s">
-        <x:v>129</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="H20" s="0" t="s">
-        <x:v>130</x:v>
+        <x:v>131</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:8">
       <x:c r="A21" s="0" t="s">
-        <x:v>131</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>132</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="C21" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>134</x:v>
       </x:c>
       <x:c r="D21" s="0" t="s">
-        <x:v>120</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="E21" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="F21" s="0" t="s">
-        <x:v>134</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="G21" s="0" t="s">
-        <x:v>135</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="H21" s="0" t="s">
-        <x:v>136</x:v>
+        <x:v>138</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:8">
       <x:c r="A22" s="0" t="s">
-        <x:v>137</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>138</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="C22" s="0" t="s">
-        <x:v>139</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="D22" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="E22" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="F22" s="0" t="s">
-        <x:v>140</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="G22" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="H22" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>144</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:8">
       <x:c r="A23" s="0" t="s">
-        <x:v>142</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>143</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="C23" s="0" t="s">
-        <x:v>144</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="D23" s="0" t="s">
-        <x:v>84</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="E23" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="F23" s="0" t="s">
-        <x:v>145</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="G23" s="0" t="s">
-        <x:v>86</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="H23" s="0" t="s">
-        <x:v>146</x:v>
+        <x:v>149</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:8">
       <x:c r="A24" s="0" t="s">
-        <x:v>147</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="C24" s="0" t="s">
-        <x:v>149</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="D24" s="0" t="s">
         <x:v>84</x:v>
@@ -1585,24 +1630,24 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F24" s="0" t="s">
-        <x:v>150</x:v>
+        <x:v>153</x:v>
       </x:c>
       <x:c r="G24" s="0" t="s">
         <x:v>86</x:v>
       </x:c>
       <x:c r="H24" s="0" t="s">
-        <x:v>151</x:v>
+        <x:v>154</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8">
       <x:c r="A25" s="0" t="s">
-        <x:v>152</x:v>
+        <x:v>155</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>153</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="C25" s="0" t="s">
-        <x:v>154</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="D25" s="0" t="s">
         <x:v>84</x:v>
@@ -1611,221 +1656,273 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F25" s="0" t="s">
-        <x:v>155</x:v>
+        <x:v>158</x:v>
       </x:c>
       <x:c r="G25" s="0" t="s">
         <x:v>86</x:v>
       </x:c>
       <x:c r="H25" s="0" t="s">
-        <x:v>156</x:v>
+        <x:v>159</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
       <x:c r="A26" s="0" t="s">
-        <x:v>157</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
-        <x:v>158</x:v>
+        <x:v>161</x:v>
       </x:c>
       <x:c r="C26" s="0" t="s">
-        <x:v>159</x:v>
+        <x:v>162</x:v>
       </x:c>
       <x:c r="D26" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="E26" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="F26" s="0" t="s">
-        <x:v>160</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="G26" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="H26" s="0" t="s">
-        <x:v>161</x:v>
+        <x:v>164</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:8">
       <x:c r="A27" s="0" t="s">
-        <x:v>162</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>166</x:v>
       </x:c>
       <x:c r="C27" s="0" t="s">
-        <x:v>164</x:v>
+        <x:v>167</x:v>
       </x:c>
       <x:c r="D27" s="0" t="s">
-        <x:v>70</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="E27" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="F27" s="0" t="s">
-        <x:v>165</x:v>
+        <x:v>168</x:v>
       </x:c>
       <x:c r="G27" s="0" t="s">
-        <x:v>166</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="H27" s="0" t="s">
-        <x:v>167</x:v>
+        <x:v>169</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
       <x:c r="A28" s="0" t="s">
-        <x:v>168</x:v>
+        <x:v>170</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
-        <x:v>169</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C28" s="0" t="s">
-        <x:v>170</x:v>
+        <x:v>172</x:v>
       </x:c>
       <x:c r="D28" s="0" t="s">
-        <x:v>102</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="E28" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="F28" s="0" t="s">
-        <x:v>171</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="G28" s="0" t="s">
-        <x:v>104</x:v>
+        <x:v>174</x:v>
       </x:c>
       <x:c r="H28" s="0" t="s">
-        <x:v>172</x:v>
+        <x:v>175</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:8">
       <x:c r="A29" s="0" t="s">
-        <x:v>173</x:v>
+        <x:v>176</x:v>
       </x:c>
       <x:c r="B29" s="0" t="s">
-        <x:v>174</x:v>
+        <x:v>177</x:v>
       </x:c>
       <x:c r="C29" s="0" t="s">
-        <x:v>175</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="D29" s="0" t="s">
-        <x:v>114</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="E29" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="F29" s="0" t="s">
-        <x:v>176</x:v>
+        <x:v>179</x:v>
       </x:c>
       <x:c r="G29" s="0" t="s">
-        <x:v>177</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="H29" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>180</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:8">
       <x:c r="A30" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>181</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>182</x:v>
       </x:c>
       <x:c r="C30" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>183</x:v>
       </x:c>
       <x:c r="D30" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="E30" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="F30" s="0" t="s">
-        <x:v>179</x:v>
+        <x:v>184</x:v>
       </x:c>
       <x:c r="G30" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>185</x:v>
       </x:c>
       <x:c r="H30" s="0" t="s">
-        <x:v>180</x:v>
+        <x:v>186</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
       <x:c r="A31" s="0" t="s">
-        <x:v>181</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
-        <x:v>182</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="C31" s="0" t="s">
-        <x:v>183</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="D31" s="0" t="s">
-        <x:v>184</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="E31" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="F31" s="0" t="s">
-        <x:v>185</x:v>
+        <x:v>187</x:v>
       </x:c>
       <x:c r="G31" s="0" t="s">
-        <x:v>92</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="H31" s="0" t="s">
-        <x:v>186</x:v>
+        <x:v>188</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:8">
       <x:c r="A32" s="0" t="s">
-        <x:v>187</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="B32" s="0" t="s">
-        <x:v>188</x:v>
+        <x:v>190</x:v>
       </x:c>
       <x:c r="C32" s="0" t="s">
-        <x:v>189</x:v>
+        <x:v>191</x:v>
       </x:c>
       <x:c r="D32" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>192</x:v>
       </x:c>
       <x:c r="E32" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="F32" s="0" t="s">
-        <x:v>190</x:v>
+        <x:v>193</x:v>
       </x:c>
       <x:c r="G32" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="H32" s="0" t="s">
-        <x:v>191</x:v>
+        <x:v>194</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8">
       <x:c r="A33" s="0" t="s">
-        <x:v>192</x:v>
+        <x:v>195</x:v>
       </x:c>
       <x:c r="B33" s="0" t="s">
-        <x:v>193</x:v>
+        <x:v>196</x:v>
       </x:c>
       <x:c r="C33" s="0" t="s">
-        <x:v>194</x:v>
+        <x:v>197</x:v>
       </x:c>
       <x:c r="D33" s="0" t="s">
-        <x:v>195</x:v>
+        <x:v>198</x:v>
       </x:c>
       <x:c r="E33" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="F33" s="0" t="s">
-        <x:v>196</x:v>
+        <x:v>199</x:v>
       </x:c>
       <x:c r="G33" s="0" t="s">
+        <x:v>200</x:v>
+      </x:c>
+      <x:c r="H33" s="0" t="s">
+        <x:v>201</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:8">
+      <x:c r="A34" s="0" t="s">
+        <x:v>202</x:v>
+      </x:c>
+      <x:c r="B34" s="0" t="s">
+        <x:v>203</x:v>
+      </x:c>
+      <x:c r="C34" s="0" t="s">
+        <x:v>204</x:v>
+      </x:c>
+      <x:c r="D34" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="E34" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="F34" s="0" t="s">
+        <x:v>205</x:v>
+      </x:c>
+      <x:c r="G34" s="0" t="s">
         <x:v>45</x:v>
       </x:c>
-      <x:c r="H33" s="0" t="s">
-        <x:v>197</x:v>
+      <x:c r="H34" s="0" t="s">
+        <x:v>206</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:8">
+      <x:c r="A35" s="0" t="s">
+        <x:v>207</x:v>
+      </x:c>
+      <x:c r="B35" s="0" t="s">
+        <x:v>208</x:v>
+      </x:c>
+      <x:c r="C35" s="0" t="s">
+        <x:v>209</x:v>
+      </x:c>
+      <x:c r="D35" s="0" t="s">
+        <x:v>210</x:v>
+      </x:c>
+      <x:c r="E35" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="F35" s="0" t="s">
+        <x:v>211</x:v>
+      </x:c>
+      <x:c r="G35" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="H35" s="0" t="s">
+        <x:v>212</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>